<commit_message>
Update port arrivals Excel
</commit_message>
<xml_diff>
--- a/output/combined_arrivals_2026-02-18.xlsx
+++ b/output/combined_arrivals_2026-02-18.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -965,7 +965,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2324,7 +2324,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3212,7 +3212,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3471,7 +3471,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3545,7 +3545,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3730,7 +3730,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3841,7 +3841,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3952,7 +3952,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4100,7 +4100,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2026-02-18 00:21</t>
+          <t>2026-02-18 00:28</t>
         </is>
       </c>
     </row>

</xml_diff>